<commit_message>
solved AB#44, fixed minor export issues related to data reloading
</commit_message>
<xml_diff>
--- a/BleRecorder.DataAccess/DataExport/TestSubjectDataExportTemplate.xlsx
+++ b/BleRecorder.DataAccess/DataExport/TestSubjectDataExportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\source\repos\mebster-com\Myodam_2.0\Mebster.Myodam.DataAccess\DataExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6432812-DD35-4560-936B-D6A5AF9B1D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9269B332-408A-4856-B3DF-1A0158D51466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{0582046B-D9DF-4D6F-9564-6C5152294F75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0582046B-D9DF-4D6F-9564-6C5152294F75}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSubject" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Maximum force [N]</t>
-  </si>
-  <si>
     <t>Mechanical adjustments</t>
   </si>
   <si>
@@ -81,6 +78,10 @@
   </si>
   <si>
     <t>First name:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum contraction [Nm] 
+/ Fatigue [%] </t>
   </si>
 </sst>
 </file>
@@ -417,7 +418,7 @@
     <tableColumn id="2" xr3:uid="{8568E63F-BAB5-402B-A587-BF55E05EA795}" name="Date" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{F1127567-43BE-4839-9245-87431D8F6F6F}" name="Measurement type" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{BEB18FB2-B1AB-40B7-9DEE-2A248EF868AE}" name="Notes" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{D84C77CD-10E2-48AE-928B-2FCDF5D11E93}" name="Maximum force [N]" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{D84C77CD-10E2-48AE-928B-2FCDF5D11E93}" name="Maximum contraction [Nm] _x000a_/ Fatigue [%] " dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{BDD03D38-CF7B-47D9-A38F-60C6526F9623}" name="Mechanical adjustments" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{A229BDE8-1A10-4FEA-979F-C82B41005F4E}" name="Stimulation parameters" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{60C85069-DEE4-480C-A75A-5801A7DDD059}" name="Measurement site" dataDxfId="1"/>
@@ -727,76 +728,76 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.54296875" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="18.54296875" customWidth="1"/>
-    <col min="4" max="4" width="39.453125" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="22.453125" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" customWidth="1"/>
-    <col min="9" max="9" width="18.7265625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="44.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="44.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="I6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="6"/>

</xml_diff>

<commit_message>
Exporting stim params into separate columns
</commit_message>
<xml_diff>
--- a/BleRecorder.DataAccess/DataExport/TestSubjectDataExportTemplate.xlsx
+++ b/BleRecorder.DataAccess/DataExport/TestSubjectDataExportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\source\repos\mebster-com\Myodam_2.0\Mebster.Myodam.DataAccess\DataExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9269B332-408A-4856-B3DF-1A0158D51466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A11895-A0D5-47B7-9E87-E83D23A60B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0582046B-D9DF-4D6F-9564-6C5152294F75}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0582046B-D9DF-4D6F-9564-6C5152294F75}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSubject" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Notes:</t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>Mechanical adjustments</t>
-  </si>
-  <si>
-    <t>Stimulation parameters</t>
-  </si>
-  <si>
-    <t>Measurement site</t>
   </si>
   <si>
     <t>Measurement type</t>
@@ -82,6 +76,27 @@
   <si>
     <t xml:space="preserve">Maximum contraction [Nm] 
 / Fatigue [%] </t>
+  </si>
+  <si>
+    <t>Stimulation current [mA]</t>
+  </si>
+  <si>
+    <t>Stimulation frequency [Hz]</t>
+  </si>
+  <si>
+    <t>Stimulation pulse width [us]</t>
+  </si>
+  <si>
+    <t>Stimulation time [s]</t>
+  </si>
+  <si>
+    <t>Rest time (fatigue) [s]</t>
+  </si>
+  <si>
+    <t>Fatigue repetitions</t>
+  </si>
+  <si>
+    <t>Leg side</t>
   </si>
 </sst>
 </file>
@@ -116,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -182,11 +197,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -210,11 +238,31 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="17">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -251,6 +299,23 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -264,6 +329,57 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -411,18 +527,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74EE6CAA-C529-430A-94D9-16302EA1513E}" name="MeasurementsTable" displayName="MeasurementsTable" ref="A6:I7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10">
-  <autoFilter ref="A6:I7" xr:uid="{74EE6CAA-C529-430A-94D9-16302EA1513E}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{57D8FD39-3008-4860-8D3A-145F94C49EBD}" name="Title" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{8568E63F-BAB5-402B-A587-BF55E05EA795}" name="Date" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{F1127567-43BE-4839-9245-87431D8F6F6F}" name="Measurement type" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{BEB18FB2-B1AB-40B7-9DEE-2A248EF868AE}" name="Notes" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{D84C77CD-10E2-48AE-928B-2FCDF5D11E93}" name="Maximum contraction [Nm] _x000a_/ Fatigue [%] " dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{BDD03D38-CF7B-47D9-A38F-60C6526F9623}" name="Mechanical adjustments" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{A229BDE8-1A10-4FEA-979F-C82B41005F4E}" name="Stimulation parameters" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{60C85069-DEE4-480C-A75A-5801A7DDD059}" name="Measurement site" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{660F4986-02FA-4494-94AE-D7877999DCFE}" name="Position during measurement" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{74EE6CAA-C529-430A-94D9-16302EA1513E}" name="MeasurementsTable" displayName="MeasurementsTable" ref="A6:N7" insertRow="1" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15">
+  <autoFilter ref="A6:N7" xr:uid="{74EE6CAA-C529-430A-94D9-16302EA1513E}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{57D8FD39-3008-4860-8D3A-145F94C49EBD}" name="Title" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{8568E63F-BAB5-402B-A587-BF55E05EA795}" name="Date" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{F1127567-43BE-4839-9245-87431D8F6F6F}" name="Measurement type" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{BEB18FB2-B1AB-40B7-9DEE-2A248EF868AE}" name="Notes" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{D84C77CD-10E2-48AE-928B-2FCDF5D11E93}" name="Maximum contraction [Nm] _x000a_/ Fatigue [%] " dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{BDD03D38-CF7B-47D9-A38F-60C6526F9623}" name="Mechanical adjustments" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{95337CC3-DE89-4A61-9650-3B36B86E751A}" name="Stimulation current [mA]" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{D9C3C387-35CD-49EC-A417-1D971892AF5D}" name="Stimulation frequency [Hz]" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{E28067C2-59C7-4027-98CC-2553BB5D1F35}" name="Stimulation pulse width [us]" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{A229BDE8-1A10-4FEA-979F-C82B41005F4E}" name="Stimulation time [s]" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{D7AED791-BE75-4167-9F8F-2113895683DE}" name="Rest time (fatigue) [s]" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{60C85069-DEE4-480C-A75A-5801A7DDD059}" name="Fatigue repetitions" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{E7C13D4E-7B98-4200-9E1C-1012AE5F6006}" name="Leg side" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{660F4986-02FA-4494-94AE-D7877999DCFE}" name="Position during measurement" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -725,79 +846,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5ECA9D1-AE27-4787-90F5-62D841C61699}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="4" max="4" width="39.453125" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="7" max="13" width="14.1796875" customWidth="1"/>
+    <col min="14" max="14" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="5"/>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:9" ht="44.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="44.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="6"/>
@@ -807,6 +942,11 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed theme to light, increased font size overall UI markup refactoring implemented AB#62
</commit_message>
<xml_diff>
--- a/BleRecorder.DataAccess/DataExport/TestSubjectDataExportTemplate.xlsx
+++ b/BleRecorder.DataAccess/DataExport/TestSubjectDataExportTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\source\repos\mebster-com\Myodam_2.0\Mebster.Myodam.DataAccess\DataExport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\mebster-com\Myodam_2.0\Mebster.Myodam.DataAccess\DataExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A11895-A0D5-47B7-9E87-E83D23A60B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B79F732-B256-4F83-803A-55E0FEE10EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0582046B-D9DF-4D6F-9564-6C5152294F75}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{0582046B-D9DF-4D6F-9564-6C5152294F75}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSubject" sheetId="1" r:id="rId1"/>
@@ -74,29 +74,29 @@
     <t>First name:</t>
   </si>
   <si>
-    <t xml:space="preserve">Maximum contraction [Nm] 
+    <t>Stimulation current [mA]</t>
+  </si>
+  <si>
+    <t>Stimulation frequency [Hz]</t>
+  </si>
+  <si>
+    <t>Stimulation pulse width [us]</t>
+  </si>
+  <si>
+    <t>Stimulation time [s]</t>
+  </si>
+  <si>
+    <t>Rest time (fatigue) [s]</t>
+  </si>
+  <si>
+    <t>Fatigue repetitions</t>
+  </si>
+  <si>
+    <t>Leg side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum contraction [N] 
 / Fatigue [%] </t>
-  </si>
-  <si>
-    <t>Stimulation current [mA]</t>
-  </si>
-  <si>
-    <t>Stimulation frequency [Hz]</t>
-  </si>
-  <si>
-    <t>Stimulation pulse width [us]</t>
-  </si>
-  <si>
-    <t>Stimulation time [s]</t>
-  </si>
-  <si>
-    <t>Rest time (fatigue) [s]</t>
-  </si>
-  <si>
-    <t>Fatigue repetitions</t>
-  </si>
-  <si>
-    <t>Leg side</t>
   </si>
 </sst>
 </file>
@@ -248,6 +248,23 @@
   <dxfs count="17">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -261,23 +278,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -534,7 +534,7 @@
     <tableColumn id="2" xr3:uid="{8568E63F-BAB5-402B-A587-BF55E05EA795}" name="Date" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{F1127567-43BE-4839-9245-87431D8F6F6F}" name="Measurement type" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{BEB18FB2-B1AB-40B7-9DEE-2A248EF868AE}" name="Notes" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{D84C77CD-10E2-48AE-928B-2FCDF5D11E93}" name="Maximum contraction [Nm] _x000a_/ Fatigue [%] " dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{D84C77CD-10E2-48AE-928B-2FCDF5D11E93}" name="Maximum contraction [N] _x000a_/ Fatigue [%] " dataDxfId="9"/>
     <tableColumn id="7" xr3:uid="{BDD03D38-CF7B-47D9-A38F-60C6526F9623}" name="Mechanical adjustments" dataDxfId="8"/>
     <tableColumn id="12" xr3:uid="{95337CC3-DE89-4A61-9650-3B36B86E751A}" name="Stimulation current [mA]" dataDxfId="7"/>
     <tableColumn id="11" xr3:uid="{D9C3C387-35CD-49EC-A417-1D971892AF5D}" name="Stimulation frequency [Hz]" dataDxfId="6"/>
@@ -542,8 +542,8 @@
     <tableColumn id="8" xr3:uid="{A229BDE8-1A10-4FEA-979F-C82B41005F4E}" name="Stimulation time [s]" dataDxfId="4"/>
     <tableColumn id="13" xr3:uid="{D7AED791-BE75-4167-9F8F-2113895683DE}" name="Rest time (fatigue) [s]" dataDxfId="3"/>
     <tableColumn id="9" xr3:uid="{60C85069-DEE4-480C-A75A-5801A7DDD059}" name="Fatigue repetitions" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{E7C13D4E-7B98-4200-9E1C-1012AE5F6006}" name="Leg side" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{660F4986-02FA-4494-94AE-D7877999DCFE}" name="Position during measurement" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{E7C13D4E-7B98-4200-9E1C-1012AE5F6006}" name="Leg side" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{660F4986-02FA-4494-94AE-D7877999DCFE}" name="Position during measurement" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -849,7 +849,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -902,31 +902,31 @@
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="N6" s="4" t="s">
         <v>7</v>

</xml_diff>